<commit_message>
Added Log4j and few testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DBB356-B954-4F63-8405-02FD9E022235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="login_test" sheetId="1" r:id="rId3"/>
+    <sheet name="login_test" sheetId="1" r:id="rId1"/>
+    <sheet name="addToCart_Test" sheetId="2" r:id="rId2"/>
+    <sheet name="RemoveFromCart_Test" sheetId="3" r:id="rId3"/>
+    <sheet name="product_Price_Validation" sheetId="4" r:id="rId4"/>
+    <sheet name="subTotalAmountValidation" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -36,12 +40,27 @@
   <si>
     <t>Ramakotaiah</t>
   </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>redmi note 11</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>Product2</t>
+  </si>
+  <si>
+    <t>iphone 13 pro max</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,22 +70,22 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,120 +97,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -465,28 +389,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238ca09e-6a31-4ece-8b39-03e3a3fa0c90}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238CA09E-6A31-4ECE-8B39-03E3A3FA0C90}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.857142857142858" customWidth="1"/>
-    <col min="2" max="2" width="9.142857142857142" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -494,15 +418,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -514,4 +438,123 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E44E017-5D93-413D-A80B-60F70A4FDF36}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2564CA6E-4F84-42B9-AE94-997C51CC2B44}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B56604-0BD9-43E2-B525-0FF47693009F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E19FC7-4FAC-46B6-B9CC-CBEBC0929716}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>